<commit_message>
Update of Dec 3
</commit_message>
<xml_diff>
--- a/resources/IDCAM_Fiche_Activité_Journaliere..xlsx
+++ b/resources/IDCAM_Fiche_Activité_Journaliere..xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7395"/>
+    <workbookView windowWidth="28800" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="Rapport Journalier" sheetId="1" r:id="rId1"/>
@@ -156,12 +156,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="179" formatCode="hh:mm:ss"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -580,7 +581,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -654,6 +655,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -709,6 +719,15 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -833,7 +852,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -845,34 +864,34 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -957,7 +976,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -999,7 +1018,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1019,17 +1038,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1037,7 +1062,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1388,8 +1419,8 @@
   <sheetPr/>
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="14.25"/>
@@ -1691,7 +1722,7 @@
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
-      <c r="G18" s="29"/>
+      <c r="G18" s="31"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
@@ -1706,7 +1737,7 @@
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
-      <c r="G19" s="29"/>
+      <c r="G19" s="31"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
@@ -1721,7 +1752,7 @@
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
-      <c r="G20" s="29"/>
+      <c r="G20" s="31"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
@@ -1736,7 +1767,7 @@
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
-      <c r="G21" s="29"/>
+      <c r="G21" s="31"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
@@ -1746,16 +1777,29 @@
       <c r="A22" s="10">
         <v>5</v>
       </c>
-      <c r="B22" s="16"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
       <c r="F22" s="23"/>
-      <c r="G22" s="16"/>
+      <c r="G22" s="23"/>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="24"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="32"/>
     </row>
     <row r="24" ht="24.6" customHeight="1"/>
     <row r="25" ht="34.2" customHeight="1" spans="1:10">
@@ -1773,11 +1817,11 @@
       <c r="J25" s="15"/>
     </row>
     <row r="26" ht="24.6" customHeight="1" spans="1:10">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="26">
+      <c r="B26" s="27"/>
+      <c r="C26" s="28">
         <v>0</v>
       </c>
       <c r="D26" s="15"/>
@@ -1830,39 +1874,39 @@
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="27"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="27"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="29"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>